<commit_message>
Update CpUDSC, BECF, BHRbEF, and TCAMRB to use latest EIA forms
</commit_message>
<xml_diff>
--- a/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
+++ b/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\TCAMRB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\TCAMRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="EIA Table 2.13" sheetId="3" r:id="rId3"/>
     <sheet name="TCAMRB" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
@@ -97,10 +97,6 @@
     <t>Exports</t>
   </si>
   <si>
-    <t>Sources: National Energy Board of Canada; DOE, Office of Electricity Delivery and Energy Reliability, Form OE-781R, 'Annual Report of International Electric Export/Import Data,' predecessor forms.
-To estimate electricity trade with Mexico, for 2001 forward data from the California Independent System Operator are used in combination with the Form OE-781R values.</t>
-  </si>
-  <si>
     <t>Mexico and Canada Imports and Exports</t>
   </si>
   <si>
@@ -116,12 +112,6 @@
     <t>Table 2.13</t>
   </si>
   <si>
-    <t>I cannot find any source that explicitly provides the capacity of transmission lines</t>
-  </si>
-  <si>
-    <t>to/from Canada.  The closest I can find is a diagram showing the voltage ratings</t>
-  </si>
-  <si>
     <t>of the 37 main interconnections between the U.S. and Canada in kV.</t>
   </si>
   <si>
@@ -155,10 +145,20 @@
     <t>Table 2.14.  Electric Power Industry - U.S. Electricity Imports from and Electricity Exports to Canada</t>
   </si>
   <si>
-    <t>and Mexico, 2007-2017 (Megawatthours)</t>
-  </si>
-  <si>
     <t>Transmission Capacity Across Modeled Region Border (MW)</t>
+  </si>
+  <si>
+    <t>Notes: As of November 2017, the data for 2016 and going forward will be published using data from the Form EIA-111, "Quarterly Electricity Imports and Exports Report." During 2013-2015, EIA revised its approach to estimating imports from Mexico.
+Sources: 2016, U.S. Energy Information Administration, Form EIA-111, "Quarterly Electricity Imports and Exports Report"; 2006-2015 data, National Energy Board of Canada; FERC 714, Annual Electric Balancing Authority Area and Planning Report; California Energy Commission; and EIA estimates.</t>
+  </si>
+  <si>
+    <t>and Mexico, 2008-2018 (Megawatthours)</t>
+  </si>
+  <si>
+    <t>We cannot find any source that explicitly provides the capacity of transmission lines</t>
+  </si>
+  <si>
+    <t>to/from Canada.  The closest we can find is a diagram showing the voltage ratings</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -294,20 +294,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -340,9 +331,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -658,7 +646,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -707,32 +695,32 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -746,7 +734,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -819,70 +807,70 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" s="12">
-        <f>SUM('EIA Table 2.13'!D8:E10)</f>
+        <f>SUM('EIA Table 2.13'!D7:E9)</f>
         <v>5707778</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" s="12">
-        <f>SUM('EIA Table 2.13'!B8:C10)</f>
+        <f>SUM('EIA Table 2.13'!B7:C9)</f>
         <v>197082568</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="14">
         <f>B8*(B22/B21)</f>
@@ -902,7 +890,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -913,7 +901,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -923,32 +911,32 @@
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="A2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
@@ -975,260 +963,260 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="10">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B5" s="11">
-        <v>50118056</v>
+        <v>55731229</v>
       </c>
       <c r="C5" s="11">
-        <v>19559417</v>
+        <v>23614158</v>
       </c>
       <c r="D5" s="11">
-        <v>1277646</v>
+        <v>1288152</v>
       </c>
       <c r="E5" s="11">
-        <v>584175</v>
+        <v>584001</v>
       </c>
       <c r="F5" s="11">
-        <v>51395702</v>
+        <v>57019381</v>
       </c>
       <c r="G5" s="11">
-        <v>20143592</v>
+        <v>24198159</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B6" s="11">
-        <v>55731229</v>
+        <v>50870451</v>
       </c>
       <c r="C6" s="11">
-        <v>23614158</v>
+        <v>17517112</v>
       </c>
       <c r="D6" s="11">
-        <v>1288152</v>
+        <v>1320144</v>
       </c>
       <c r="E6" s="11">
-        <v>584001</v>
+        <v>620872</v>
       </c>
       <c r="F6" s="11">
-        <v>57019381</v>
+        <v>52190595</v>
       </c>
       <c r="G6" s="11">
-        <v>24198159</v>
+        <v>18137984</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="10">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B7" s="11">
-        <v>50870451</v>
+        <v>43763091</v>
       </c>
       <c r="C7" s="11">
-        <v>17517112</v>
+        <v>18481678</v>
       </c>
       <c r="D7" s="11">
-        <v>1320144</v>
+        <v>1320095</v>
       </c>
       <c r="E7" s="11">
-        <v>620872</v>
+        <v>624502</v>
       </c>
       <c r="F7" s="11">
-        <v>52190595</v>
+        <v>45083186</v>
       </c>
       <c r="G7" s="11">
-        <v>18137984</v>
+        <v>19106180</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B8" s="11">
-        <v>43763091</v>
+        <v>51075952</v>
       </c>
       <c r="C8" s="11">
-        <v>18481678</v>
+        <v>14398470</v>
       </c>
       <c r="D8" s="11">
-        <v>1320095</v>
+        <v>1223758</v>
       </c>
       <c r="E8" s="11">
-        <v>624502</v>
+        <v>650082</v>
       </c>
       <c r="F8" s="11">
-        <v>45083186</v>
+        <v>52299710</v>
       </c>
       <c r="G8" s="11">
-        <v>19106180</v>
+        <v>15048552</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="10">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B9" s="11">
-        <v>51075952</v>
+        <v>57971110</v>
       </c>
       <c r="C9" s="11">
-        <v>14398470</v>
+        <v>11392267</v>
       </c>
       <c r="D9" s="11">
-        <v>1223758</v>
+        <v>1285959</v>
       </c>
       <c r="E9" s="11">
-        <v>650082</v>
+        <v>603382</v>
       </c>
       <c r="F9" s="11">
-        <v>52299710</v>
+        <v>59257069</v>
       </c>
       <c r="G9" s="11">
-        <v>15048552</v>
+        <v>11995649</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="10">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B10" s="11">
-        <v>57971110</v>
+        <v>62739038</v>
       </c>
       <c r="C10" s="11">
-        <v>11392267</v>
+        <v>10694907</v>
       </c>
       <c r="D10" s="11">
-        <v>1285959</v>
+        <v>6207597</v>
       </c>
       <c r="E10" s="11">
-        <v>603382</v>
+        <v>678300</v>
       </c>
       <c r="F10" s="11">
-        <v>59257069</v>
+        <v>68946635</v>
       </c>
       <c r="G10" s="11">
-        <v>11995649</v>
+        <v>11373207</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="10">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B11" s="11">
-        <v>62739038</v>
+        <v>59369660</v>
       </c>
       <c r="C11" s="11">
-        <v>10694907</v>
+        <v>12860889</v>
       </c>
       <c r="D11" s="11">
-        <v>6207597</v>
+        <v>7140624</v>
       </c>
       <c r="E11" s="11">
-        <v>678300</v>
+        <v>437364</v>
       </c>
       <c r="F11" s="11">
-        <v>68946635</v>
+        <v>66510284</v>
       </c>
       <c r="G11" s="11">
-        <v>11373207</v>
+        <v>13298253</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B12" s="11">
-        <v>59369660</v>
+        <v>68462277</v>
       </c>
       <c r="C12" s="11">
-        <v>12860889</v>
+        <v>8707873</v>
       </c>
       <c r="D12" s="11">
-        <v>7140624</v>
+        <v>7308192</v>
       </c>
       <c r="E12" s="11">
-        <v>437364</v>
+        <v>392016</v>
       </c>
       <c r="F12" s="11">
-        <v>66510284</v>
+        <v>75770469</v>
       </c>
       <c r="G12" s="11">
-        <v>13298253</v>
+        <v>9099889</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="10">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B13" s="11">
-        <v>68462277</v>
+        <v>65173818</v>
       </c>
       <c r="C13" s="11">
-        <v>8707873</v>
+        <v>2682381</v>
       </c>
       <c r="D13" s="11">
-        <v>7308192</v>
+        <v>7542445</v>
       </c>
       <c r="E13" s="11">
-        <v>392016</v>
+        <v>3531636</v>
       </c>
       <c r="F13" s="11">
-        <v>75770469</v>
+        <v>72716263</v>
       </c>
       <c r="G13" s="11">
-        <v>9099889</v>
+        <v>6214017</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B14" s="11">
-        <v>65173818</v>
+        <v>59909320</v>
       </c>
       <c r="C14" s="11">
-        <v>2682381</v>
+        <v>3312798</v>
       </c>
       <c r="D14" s="11">
-        <v>7542445</v>
+        <v>5775597</v>
       </c>
       <c r="E14" s="11">
-        <v>3531636</v>
+        <v>6058005</v>
       </c>
       <c r="F14" s="11">
-        <v>72716263</v>
+        <v>65684917</v>
       </c>
       <c r="G14" s="11">
-        <v>6214017</v>
+        <v>9370803</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="10">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B15" s="11">
-        <v>59909320</v>
+        <v>51494627</v>
       </c>
       <c r="C15" s="11">
-        <v>3312798</v>
+        <v>7290070</v>
       </c>
       <c r="D15" s="11">
-        <v>5775597</v>
+        <v>6765975</v>
       </c>
       <c r="E15" s="11">
-        <v>6058005</v>
+        <v>6514422</v>
       </c>
       <c r="F15" s="11">
-        <v>65684917</v>
+        <v>58260602</v>
       </c>
       <c r="G15" s="11">
-        <v>9370803</v>
+        <v>13804492</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1265,7 +1253,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updates for more recent EIA data
</commit_message>
<xml_diff>
--- a/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
+++ b/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\TCAMRB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\TCAMRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85707D12-8168-4B0C-BC6F-75CC4FE54955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="23955" windowHeight="12855"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,18 @@
     <sheet name="EIA Table 2.13" sheetId="3" r:id="rId3"/>
     <sheet name="TCAMRB" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,12 +115,6 @@
     <t>Energy Information Administration</t>
   </si>
   <si>
-    <t>Electric Power Annual</t>
-  </si>
-  <si>
-    <t>http://www.eia.gov/electricity/annual/xls/epa_02_13.xlsx</t>
-  </si>
-  <si>
     <t>Table 2.13</t>
   </si>
   <si>
@@ -148,23 +154,29 @@
     <t>Transmission Capacity Across Modeled Region Border (MW)</t>
   </si>
   <si>
+    <t>We cannot find any source that explicitly provides the capacity of transmission lines</t>
+  </si>
+  <si>
+    <t>to/from Canada.  The closest we can find is a diagram showing the voltage ratings</t>
+  </si>
+  <si>
+    <t>and Mexico, 2009-2019 (Megawatthours)</t>
+  </si>
+  <si>
     <t>Notes: As of November 2017, the data for 2016 and going forward will be published using data from the Form EIA-111, "Quarterly Electricity Imports and Exports Report." During 2013-2015, EIA revised its approach to estimating imports from Mexico.
-Sources: 2016, U.S. Energy Information Administration, Form EIA-111, "Quarterly Electricity Imports and Exports Report"; 2006-2015 data, National Energy Board of Canada; FERC 714, Annual Electric Balancing Authority Area and Planning Report; California Energy Commission; and EIA estimates.</t>
-  </si>
-  <si>
-    <t>and Mexico, 2008-2018 (Megawatthours)</t>
-  </si>
-  <si>
-    <t>We cannot find any source that explicitly provides the capacity of transmission lines</t>
-  </si>
-  <si>
-    <t>to/from Canada.  The closest we can find is a diagram showing the voltage ratings</t>
+Sources: 2016-2019, U.S. Energy Information Administration, Form EIA-111, "Quarterly Electricity Imports and Exports Report"; 2006-2015 data, National Energy Board of Canada; FERC 714, Annual Electric Balancing Authority Area and Planning Report; California Energy Commission; and EIA estimates.</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/electricity/annual/</t>
+  </si>
+  <si>
+    <t>Electric Power Annual 2020 (with data for 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -311,34 +323,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,6 +445,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -467,6 +497,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,25 +689,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.265625" customWidth="1"/>
-    <col min="2" max="2" width="70.265625" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="70.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -668,59 +715,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -730,25 +777,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.73046875" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -756,7 +803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -764,7 +811,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -772,7 +819,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -780,7 +827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -788,7 +835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -796,7 +843,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -805,76 +852,76 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="6" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="8">
+        <f>SUM('EIA Table 2.13'!D7:E9)</f>
+        <v>10649078</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="8">
+        <f>SUM('EIA Table 2.13'!B7:C9)</f>
+        <v>208271744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="12">
-        <f>SUM('EIA Table 2.13'!D7:E9)</f>
-        <v>5707778</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="12">
-        <f>SUM('EIA Table 2.13'!B7:C9)</f>
-        <v>197082568</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="14">
+      <c r="B24" s="10">
         <f>B8*(B22/B21)</f>
-        <v>44404.001425423347</v>
+        <v>25151.234950481161</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
@@ -886,344 +933,344 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="17.1328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="7"/>
+    <col min="1" max="7" width="17.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.08984375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="17">
+        <v>2009</v>
+      </c>
+      <c r="B5" s="18">
+        <v>50870451</v>
+      </c>
+      <c r="C5" s="18">
+        <v>17517112</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1320144</v>
+      </c>
+      <c r="E5" s="18">
+        <v>620872</v>
+      </c>
+      <c r="F5" s="18">
+        <v>52190595</v>
+      </c>
+      <c r="G5" s="18">
+        <v>18137984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="17">
+        <v>2010</v>
+      </c>
+      <c r="B6" s="18">
+        <v>43763091</v>
+      </c>
+      <c r="C6" s="18">
+        <v>18481678</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1320095</v>
+      </c>
+      <c r="E6" s="18">
+        <v>624502</v>
+      </c>
+      <c r="F6" s="18">
+        <v>45083186</v>
+      </c>
+      <c r="G6" s="18">
+        <v>19106180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>2011</v>
+      </c>
+      <c r="B7" s="18">
+        <v>51075952</v>
+      </c>
+      <c r="C7" s="18">
+        <v>14398470</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1223758</v>
+      </c>
+      <c r="E7" s="18">
+        <v>650082</v>
+      </c>
+      <c r="F7" s="18">
+        <v>52299710</v>
+      </c>
+      <c r="G7" s="18">
+        <v>15048552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="17">
+        <v>2012</v>
+      </c>
+      <c r="B8" s="18">
+        <v>57971110</v>
+      </c>
+      <c r="C8" s="18">
+        <v>11392267</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1285959</v>
+      </c>
+      <c r="E8" s="18">
+        <v>603382</v>
+      </c>
+      <c r="F8" s="18">
+        <v>59257069</v>
+      </c>
+      <c r="G8" s="18">
+        <v>11995649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
+        <v>2013</v>
+      </c>
+      <c r="B9" s="18">
+        <v>62739038</v>
+      </c>
+      <c r="C9" s="18">
+        <v>10694907</v>
+      </c>
+      <c r="D9" s="18">
+        <v>6207597</v>
+      </c>
+      <c r="E9" s="18">
+        <v>678300</v>
+      </c>
+      <c r="F9" s="18">
+        <v>68946635</v>
+      </c>
+      <c r="G9" s="18">
+        <v>11373207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="17">
+        <v>2014</v>
+      </c>
+      <c r="B10" s="18">
+        <v>59369660</v>
+      </c>
+      <c r="C10" s="18">
+        <v>12860889</v>
+      </c>
+      <c r="D10" s="18">
+        <v>7140624</v>
+      </c>
+      <c r="E10" s="18">
+        <v>437364</v>
+      </c>
+      <c r="F10" s="18">
+        <v>66510284</v>
+      </c>
+      <c r="G10" s="18">
+        <v>13298253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="17">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="18">
+        <v>68462277</v>
+      </c>
+      <c r="C11" s="18">
+        <v>8707873</v>
+      </c>
+      <c r="D11" s="18">
+        <v>7308192</v>
+      </c>
+      <c r="E11" s="18">
+        <v>392016</v>
+      </c>
+      <c r="F11" s="18">
+        <v>75770469</v>
+      </c>
+      <c r="G11" s="18">
+        <v>9099889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="17">
+        <v>2016</v>
+      </c>
+      <c r="B12" s="18">
+        <v>65173818</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2682381</v>
+      </c>
+      <c r="D12" s="18">
+        <v>7542445</v>
+      </c>
+      <c r="E12" s="18">
+        <v>3531636</v>
+      </c>
+      <c r="F12" s="18">
+        <v>72716263</v>
+      </c>
+      <c r="G12" s="18">
+        <v>6214017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
+        <v>2017</v>
+      </c>
+      <c r="B13" s="18">
+        <v>59909320</v>
+      </c>
+      <c r="C13" s="18">
+        <v>3312798</v>
+      </c>
+      <c r="D13" s="18">
+        <v>5775597</v>
+      </c>
+      <c r="E13" s="18">
+        <v>6058005</v>
+      </c>
+      <c r="F13" s="18">
+        <v>65684917</v>
+      </c>
+      <c r="G13" s="18">
+        <v>9370803</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
+        <v>2018</v>
+      </c>
+      <c r="B14" s="18">
+        <v>51494627</v>
+      </c>
+      <c r="C14" s="18">
+        <v>7290070</v>
+      </c>
+      <c r="D14" s="18">
+        <v>6765975</v>
+      </c>
+      <c r="E14" s="18">
+        <v>6514422</v>
+      </c>
+      <c r="F14" s="18">
+        <v>58260602</v>
+      </c>
+      <c r="G14" s="18">
+        <v>13804492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
+        <v>2019</v>
+      </c>
+      <c r="B15" s="18">
+        <v>52309254</v>
+      </c>
+      <c r="C15" s="18">
+        <v>13532067</v>
+      </c>
+      <c r="D15" s="18">
+        <v>6743207</v>
+      </c>
+      <c r="E15" s="18">
+        <v>6475965</v>
+      </c>
+      <c r="F15" s="18">
+        <v>59052461</v>
+      </c>
+      <c r="G15" s="18">
+        <v>20008032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="20" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="1:7" ht="26.65" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="10">
-        <v>2008</v>
-      </c>
-      <c r="B5" s="11">
-        <v>55731229</v>
-      </c>
-      <c r="C5" s="11">
-        <v>23614158</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1288152</v>
-      </c>
-      <c r="E5" s="11">
-        <v>584001</v>
-      </c>
-      <c r="F5" s="11">
-        <v>57019381</v>
-      </c>
-      <c r="G5" s="11">
-        <v>24198159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="10">
-        <v>2009</v>
-      </c>
-      <c r="B6" s="11">
-        <v>50870451</v>
-      </c>
-      <c r="C6" s="11">
-        <v>17517112</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1320144</v>
-      </c>
-      <c r="E6" s="11">
-        <v>620872</v>
-      </c>
-      <c r="F6" s="11">
-        <v>52190595</v>
-      </c>
-      <c r="G6" s="11">
-        <v>18137984</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="10">
-        <v>2010</v>
-      </c>
-      <c r="B7" s="11">
-        <v>43763091</v>
-      </c>
-      <c r="C7" s="11">
-        <v>18481678</v>
-      </c>
-      <c r="D7" s="11">
-        <v>1320095</v>
-      </c>
-      <c r="E7" s="11">
-        <v>624502</v>
-      </c>
-      <c r="F7" s="11">
-        <v>45083186</v>
-      </c>
-      <c r="G7" s="11">
-        <v>19106180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="10">
-        <v>2011</v>
-      </c>
-      <c r="B8" s="11">
-        <v>51075952</v>
-      </c>
-      <c r="C8" s="11">
-        <v>14398470</v>
-      </c>
-      <c r="D8" s="11">
-        <v>1223758</v>
-      </c>
-      <c r="E8" s="11">
-        <v>650082</v>
-      </c>
-      <c r="F8" s="11">
-        <v>52299710</v>
-      </c>
-      <c r="G8" s="11">
-        <v>15048552</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="10">
-        <v>2012</v>
-      </c>
-      <c r="B9" s="11">
-        <v>57971110</v>
-      </c>
-      <c r="C9" s="11">
-        <v>11392267</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1285959</v>
-      </c>
-      <c r="E9" s="11">
-        <v>603382</v>
-      </c>
-      <c r="F9" s="11">
-        <v>59257069</v>
-      </c>
-      <c r="G9" s="11">
-        <v>11995649</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B10" s="11">
-        <v>62739038</v>
-      </c>
-      <c r="C10" s="11">
-        <v>10694907</v>
-      </c>
-      <c r="D10" s="11">
-        <v>6207597</v>
-      </c>
-      <c r="E10" s="11">
-        <v>678300</v>
-      </c>
-      <c r="F10" s="11">
-        <v>68946635</v>
-      </c>
-      <c r="G10" s="11">
-        <v>11373207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B11" s="11">
-        <v>59369660</v>
-      </c>
-      <c r="C11" s="11">
-        <v>12860889</v>
-      </c>
-      <c r="D11" s="11">
-        <v>7140624</v>
-      </c>
-      <c r="E11" s="11">
-        <v>437364</v>
-      </c>
-      <c r="F11" s="11">
-        <v>66510284</v>
-      </c>
-      <c r="G11" s="11">
-        <v>13298253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B12" s="11">
-        <v>68462277</v>
-      </c>
-      <c r="C12" s="11">
-        <v>8707873</v>
-      </c>
-      <c r="D12" s="11">
-        <v>7308192</v>
-      </c>
-      <c r="E12" s="11">
-        <v>392016</v>
-      </c>
-      <c r="F12" s="11">
-        <v>75770469</v>
-      </c>
-      <c r="G12" s="11">
-        <v>9099889</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B13" s="11">
-        <v>65173818</v>
-      </c>
-      <c r="C13" s="11">
-        <v>2682381</v>
-      </c>
-      <c r="D13" s="11">
-        <v>7542445</v>
-      </c>
-      <c r="E13" s="11">
-        <v>3531636</v>
-      </c>
-      <c r="F13" s="11">
-        <v>72716263</v>
-      </c>
-      <c r="G13" s="11">
-        <v>6214017</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B14" s="11">
-        <v>59909320</v>
-      </c>
-      <c r="C14" s="11">
-        <v>3312798</v>
-      </c>
-      <c r="D14" s="11">
-        <v>5775597</v>
-      </c>
-      <c r="E14" s="11">
-        <v>6058005</v>
-      </c>
-      <c r="F14" s="11">
-        <v>65684917</v>
-      </c>
-      <c r="G14" s="11">
-        <v>9370803</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="10">
-        <v>2018</v>
-      </c>
-      <c r="B15" s="11">
-        <v>51494627</v>
-      </c>
-      <c r="C15" s="11">
-        <v>7290070</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6765975</v>
-      </c>
-      <c r="E15" s="11">
-        <v>6514422</v>
-      </c>
-      <c r="F15" s="11">
-        <v>58260602</v>
-      </c>
-      <c r="G15" s="11">
-        <v>13804492</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1239,7 +1286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1249,20 +1296,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="9">
         <f>SUM(Calculations!B8,Calculations!B24)</f>
-        <v>45690.001425423347</v>
+        <v>26437.234950481161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AEO 2023 TCAMRB updates
</commit_message>
<xml_diff>
--- a/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
+++ b/InputData/elec/TCAMRB/Trans Cap Across Modeled Region Border.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\TCAMRB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-us\InputData\elec\TCAMRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478447AC-9F44-4476-A790-5463A10EC44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB23C4E-5A2C-4401-9A8C-FFC0E464E98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="-5760" windowWidth="19410" windowHeight="20985" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -160,24 +160,24 @@
     <t>https://www.eia.gov/electricity/annual/</t>
   </si>
   <si>
-    <t>and Mexico, 2010-2020 (Megawatthours)</t>
+    <t>Table 2.14</t>
+  </si>
+  <si>
+    <t>and Mexico, 2011-2021 (Megawatthours)</t>
   </si>
   <si>
     <t>Notes: As of November 2017, the data for 2016 and going forward will be published using data from the Form EIA-111, "Quarterly Electricity Imports and Exports Report." During 2013-2015, EIA revised its approach to estimating imports from Mexico.
-Sources: 2016-2020, U.S. Energy Information Administration, Form EIA-111, "Quarterly Electricity Imports and Exports Report"; 2006-2015 data, National Energy Board of Canada; FERC 714, Annual Electric Balancing Authority Area and Planning Report; California Energy Commission; and EIA estimates.</t>
-  </si>
-  <si>
-    <t>Table 2.14</t>
-  </si>
-  <si>
-    <t>Electric Power Annual 2021 (with data for 2020)</t>
+Sources: 2016-2021, U.S. Energy Information Administration, Form EIA-111, "Quarterly Electricity Imports and Exports Report"; 2006-2015 data, National Energy Board of Canada; FERC 714, Annual Electric Balancing Authority Area and Planning Report; California Energy Commission; and EIA estimates.</t>
+  </si>
+  <si>
+    <t>Electric Power Annual 2022 (with data for 2021)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,31 +194,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="30"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -226,8 +201,148 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="30"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,8 +379,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -314,12 +602,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,42 +766,81 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="25" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="28" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="31" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="34" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="26" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="29" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="32" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="35" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1 2" xfId="37" xr:uid="{22928FDD-DB72-44D1-8734-F83EF9E34890}"/>
+    <cellStyle name="60% - Accent2 2" xfId="38" xr:uid="{B4DC534A-EAA7-4371-8CCC-E42962D1BF8D}"/>
+    <cellStyle name="60% - Accent3 2" xfId="39" xr:uid="{2966287B-452A-4806-BADC-9864BEC67821}"/>
+    <cellStyle name="60% - Accent4 2" xfId="40" xr:uid="{53F01230-4BDD-4947-A108-E6CF3D8CF61C}"/>
+    <cellStyle name="60% - Accent5 2" xfId="41" xr:uid="{F2DAD59C-19C7-4DDF-9F9E-6220B2DC75AC}"/>
+    <cellStyle name="60% - Accent6 2" xfId="42" xr:uid="{D4EFF933-BE32-445F-A73A-C8D8D67DC2AC}"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="21" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="24" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="27" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="30" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="33" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="36" xr:uid="{1393ABE0-B5F8-436B-8089-092930554B9F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -703,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +1238,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -772,13 +1247,13 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +1270,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,22 +1342,22 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -915,27 +1390,27 @@
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <f>SUM('EIA Table 2.14'!D5:E7)</f>
-        <v>5707778</v>
+        <v>10649078</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <f>SUM('EIA Table 2.14'!B5:C7)</f>
-        <v>197082568</v>
+        <v>208271744</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <f>B8*(B22/B21)</f>
-        <v>44404.001425423347</v>
+        <v>25151.234950481161</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
@@ -951,340 +1426,340 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="17.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.08984375" style="7"/>
+    <col min="1" max="7" width="17.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.08984375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
-        <v>2010</v>
-      </c>
-      <c r="B5" s="15">
-        <v>43763091</v>
-      </c>
-      <c r="C5" s="15">
-        <v>18481678</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1320095</v>
-      </c>
-      <c r="E5" s="15">
-        <v>624502</v>
-      </c>
-      <c r="F5" s="15">
-        <v>45083186</v>
-      </c>
-      <c r="G5" s="15">
-        <v>19106180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="18">
         <v>2011</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B5" s="19">
         <v>51075952</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C5" s="19">
         <v>14398470</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D5" s="19">
         <v>1223758</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E5" s="19">
         <v>650082</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F5" s="19">
         <v>52299710</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G5" s="19">
         <v>15048552</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="18">
         <v>2012</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B6" s="19">
         <v>57971110</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C6" s="19">
         <v>11392267</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D6" s="19">
         <v>1285959</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E6" s="19">
         <v>603382</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F6" s="19">
         <v>59257069</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G6" s="19">
         <v>11995649</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="18">
         <v>2013</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B7" s="19">
         <v>62739038</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C7" s="19">
         <v>10694907</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D7" s="19">
         <v>6207597</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E7" s="19">
         <v>678300</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F7" s="19">
         <v>68946635</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G7" s="19">
         <v>11373207</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
         <v>2014</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B8" s="19">
         <v>59369660</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C8" s="19">
         <v>12860889</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D8" s="19">
         <v>7140624</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E8" s="19">
         <v>437364</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F8" s="19">
         <v>66510284</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G8" s="19">
         <v>13298253</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="18">
         <v>2015</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B9" s="19">
         <v>68462277</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C9" s="19">
         <v>8707873</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D9" s="19">
         <v>7308192</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E9" s="19">
         <v>392016</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F9" s="19">
         <v>75770469</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G9" s="19">
         <v>9099889</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="18">
         <v>2016</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B10" s="19">
         <v>65173818</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C10" s="19">
         <v>2682381</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D10" s="19">
         <v>7542445</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E10" s="19">
         <v>3531636</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F10" s="19">
         <v>72716263</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G10" s="19">
         <v>6214017</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="18">
         <v>2017</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B11" s="19">
         <v>59909320</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C11" s="19">
         <v>3312798</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D11" s="19">
         <v>5775597</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E11" s="19">
         <v>6058005</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F11" s="19">
         <v>65684917</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G11" s="19">
         <v>9370803</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="18">
         <v>2018</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B12" s="19">
         <v>51494627</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C12" s="19">
         <v>7290070</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D12" s="19">
         <v>6765975</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E12" s="19">
         <v>6514422</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F12" s="19">
         <v>58260602</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G12" s="19">
         <v>13804492</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="18">
         <v>2019</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B13" s="19">
         <v>52309254</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C13" s="19">
         <v>13532067</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D13" s="19">
         <v>6743207</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E13" s="19">
         <v>6475965</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F13" s="19">
         <v>59052461</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G13" s="19">
         <v>20008032</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="18">
         <v>2020</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B14" s="19">
         <v>57001240</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C14" s="19">
         <v>9855106</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D14" s="19">
         <v>4447623</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E14" s="19">
         <v>4279573</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F14" s="19">
         <v>61448863</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G14" s="19">
         <v>14134679</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="18">
+        <v>2021</v>
+      </c>
+      <c r="B15" s="19">
+        <v>48140438</v>
+      </c>
+      <c r="C15" s="19">
+        <v>10067396</v>
+      </c>
+      <c r="D15" s="19">
+        <v>5026570</v>
+      </c>
+      <c r="E15" s="19">
+        <v>3788022</v>
+      </c>
+      <c r="F15" s="19">
+        <v>53167008</v>
+      </c>
+      <c r="G15" s="19">
+        <v>13855418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1306,8 +1781,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1321,9 +1796,9 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <f>SUM(Calculations!B8,Calculations!B24)</f>
-        <v>45690.001425423347</v>
+        <v>26437.234950481161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>